<commit_message>
fix lef side asignment on ready dcm common js
</commit_message>
<xml_diff>
--- a/public_html/docs/users.xlsx
+++ b/public_html/docs/users.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DarwinAlejandro\Documents\NetBeansProjects\portal-uce\public_html\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtic\Documents\GitHub\NetBeansProjects\portal-uce\public_html\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
   <si>
     <t>dsono</t>
   </si>
@@ -372,13 +372,55 @@
     <t>UCE</t>
   </si>
   <si>
-    <t>Comunicación y cultura</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>/w/direcs/comunicación-y-cultura</t>
+    <t>Artes</t>
+  </si>
+  <si>
+    <t>Arquitectura y Urbanismo</t>
+  </si>
+  <si>
+    <t>Ciencias Administrativas</t>
+  </si>
+  <si>
+    <t>Ciencias Agrícolas</t>
+  </si>
+  <si>
+    <t>Ciencias Económicas</t>
+  </si>
+  <si>
+    <t>Ciencias Médicas</t>
+  </si>
+  <si>
+    <t>Ciencias Psicológicas</t>
+  </si>
+  <si>
+    <t>Ciencias Químicas</t>
+  </si>
+  <si>
+    <t>Comunicación Social</t>
+  </si>
+  <si>
+    <t>Cultura Física</t>
+  </si>
+  <si>
+    <t>Ingeniería Ciencias Físicas y Matemática</t>
+  </si>
+  <si>
+    <t>Filosofía, Letras y Ciencias de la Educación</t>
+  </si>
+  <si>
+    <t>Ingeniería en Geología, Minas, Petróleo y Ambiental</t>
+  </si>
+  <si>
+    <t>Ingeniería Química</t>
+  </si>
+  <si>
+    <t>Jurisprudencia, Ciencias Políticas y Sociales</t>
+  </si>
+  <si>
+    <t>Medicina Veterinaria y Zootecnia</t>
+  </si>
+  <si>
+    <t>Odontología</t>
   </si>
 </sst>
 </file>
@@ -699,7 +741,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,15 +1225,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" bestFit="1" customWidth="1"/>
@@ -1232,21 +1274,168 @@
       <c r="B3" t="s">
         <v>115</v>
       </c>
-      <c r="C3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add panel collapside slide
</commit_message>
<xml_diff>
--- a/public_html/docs/users.xlsx
+++ b/public_html/docs/users.xlsx
@@ -979,7 +979,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,7 +2166,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C38" t="s">
         <v>148</v>
@@ -2175,11 +2175,7 @@
         <v>151</v>
       </c>
       <c r="E38" t="s">
-        <v>204</v>
-      </c>
-      <c r="G38" t="str">
-        <f>Users!C28</f>
-        <v>crsalas@uce.edu.ec</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2187,7 +2183,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C39" t="s">
         <v>148</v>
@@ -2196,36 +2192,36 @@
         <v>151</v>
       </c>
       <c r="E39" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>141</v>
-      </c>
-      <c r="C40" t="s">
-        <v>148</v>
-      </c>
-      <c r="D40" t="s">
-        <v>151</v>
-      </c>
-      <c r="E40" t="s">
         <v>206</v>
       </c>
-      <c r="G40" t="str">
+      <c r="G39" t="str">
         <f>Users!C24</f>
         <v>caortiz@uce.edu.ec</v>
       </c>
     </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
         <v>148</v>
@@ -2234,15 +2230,15 @@
         <v>152</v>
       </c>
       <c r="E42" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C43" t="s">
         <v>148</v>
@@ -2251,15 +2247,15 @@
         <v>152</v>
       </c>
       <c r="E43" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s">
         <v>148</v>
@@ -2268,15 +2264,15 @@
         <v>152</v>
       </c>
       <c r="E44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C45" t="s">
         <v>148</v>
@@ -2285,41 +2281,45 @@
         <v>152</v>
       </c>
       <c r="E45" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>146</v>
-      </c>
-      <c r="C46" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>43</v>
+      </c>
+      <c r="B47" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" t="s">
         <v>148</v>
       </c>
-      <c r="D46" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" t="s">
-        <v>158</v>
+      <c r="D47" t="s">
+        <v>168</v>
+      </c>
+      <c r="E47" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="C48" t="s">
         <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s">
-        <v>169</v>
+        <v>204</v>
+      </c>
+      <c r="G48" t="str">
+        <f>Users!C28</f>
+        <v>crsalas@uce.edu.ec</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update docs, fixed direcciones nombre, fixed dockbar
</commit_message>
<xml_diff>
--- a/public_html/docs/users.xlsx
+++ b/public_html/docs/users.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,6 +1760,9 @@
       <c r="G6" t="str">
         <f>Users!C6</f>
         <v>cendara@uce.edu.ec</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update sharex on noti
</commit_message>
<xml_diff>
--- a/public_html/docs/users.xlsx
+++ b/public_html/docs/users.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -1058,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1610,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix file without seguimiento
</commit_message>
<xml_diff>
--- a/public_html/docs/users.xlsx
+++ b/public_html/docs/users.xlsx
@@ -1610,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>